<commit_message>
Update Invoice Log and now dropping entries with no Reported Customer.
</commit_message>
<xml_diff>
--- a/Mill-Max Invoice Log.xlsx
+++ b/Mill-Max Invoice Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atrev\OneDrive\Documents\GitHub\TAARCOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\GitHub\TAARCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>Customer</t>
   </si>
@@ -156,9 +156,6 @@
     <t>9050-0-00-15-00-00-33-0</t>
   </si>
   <si>
-    <t>ERC Concepts</t>
-  </si>
-  <si>
     <t>854-22-005-40-001101</t>
   </si>
   <si>
@@ -176,6 +173,33 @@
   <si>
     <t>4368-0-00-34-00-00-33-0</t>
   </si>
+  <si>
+    <t>Wjr Inc.</t>
+  </si>
+  <si>
+    <t>2506-2-00-15-00-00-07-0</t>
+  </si>
+  <si>
+    <t>S 992-43-008-32-590000</t>
+  </si>
+  <si>
+    <t>70580-00-13-00-00-33-0</t>
+  </si>
+  <si>
+    <t>892-22-001-20-810000</t>
+  </si>
+  <si>
+    <t>2036-0-57-15-00-00-03-0</t>
+  </si>
+  <si>
+    <t>Chalgren Enterprises</t>
+  </si>
+  <si>
+    <t>43580-00-15-00-00-38-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERC Concepts </t>
+  </si>
 </sst>
 </file>
 
@@ -185,7 +209,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -210,8 +234,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,8 +275,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -246,85 +291,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -341,14 +311,59 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -360,8 +375,8 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -370,79 +385,115 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,34 +501,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -682,19 +705,47 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
+        </left>
+        <right style="thin">
           <color rgb="FF000000"/>
-        </bottom>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -711,14 +762,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E55" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="6" tableBorderDxfId="7">
-  <autoFilter ref="A1:E55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E123" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="A1:E123"/>
+  <sortState ref="A2:E123">
+    <sortCondition descending="1" ref="C1:C123"/>
+  </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="Customer" dataDxfId="5"/>
-    <tableColumn id="2" name="Date" dataDxfId="4"/>
-    <tableColumn id="3" name="Inv#" dataDxfId="3"/>
-    <tableColumn id="4" name="Part Number" dataDxfId="2"/>
-    <tableColumn id="5" name="inv$" dataDxfId="1"/>
+    <tableColumn id="1" name="Customer" dataDxfId="4"/>
+    <tableColumn id="2" name="Date" dataDxfId="3"/>
+    <tableColumn id="3" name="Inv#" dataDxfId="2"/>
+    <tableColumn id="4" name="Part Number" dataDxfId="1"/>
+    <tableColumn id="5" name="inv$" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -989,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1005,362 +1059,362 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="8">
+        <v>43461</v>
+      </c>
+      <c r="C2" s="7">
+        <v>933085</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="9">
+        <v>2183.6</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8">
+        <v>43437</v>
+      </c>
+      <c r="C3" s="7">
+        <v>931722</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1435</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="8">
+        <v>43433</v>
+      </c>
+      <c r="C4" s="7">
+        <v>931446</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2183</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="8">
+        <v>43432</v>
+      </c>
+      <c r="C5" s="7">
+        <v>931370</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="9">
+        <v>15500</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8">
+        <v>43434</v>
+      </c>
+      <c r="C6" s="7">
+        <v>931531</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="9">
+        <v>9471</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="11">
+        <v>43397</v>
+      </c>
+      <c r="C7" s="10">
+        <v>929279</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="12">
+        <v>5995</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="11">
+        <v>43390</v>
+      </c>
+      <c r="C8" s="10">
+        <v>928786</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="12">
+        <v>2843.4</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="11">
+        <v>43382</v>
+      </c>
+      <c r="C9" s="10">
+        <v>928146</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1500</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="11">
+        <v>43384</v>
+      </c>
+      <c r="C10" s="10">
+        <v>928276</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="12">
+        <v>9471</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="11">
+        <v>43374</v>
+      </c>
+      <c r="C11" s="10">
+        <v>927655</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="12">
+        <v>1435</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11">
+        <v>43370</v>
+      </c>
+      <c r="C12" s="10">
+        <v>927414</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="12">
+        <v>8230</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <v>43370</v>
+      </c>
+      <c r="C13" s="10">
+        <v>927453</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="12">
+        <v>7500</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="11">
+        <v>43367</v>
+      </c>
+      <c r="C14" s="10">
+        <v>927071</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="12">
+        <v>1408.5</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="11">
+        <v>43363</v>
+      </c>
+      <c r="C15" s="10">
+        <v>926825</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="12">
+        <v>13346.96</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B16" s="11">
         <v>43357</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C16" s="10">
         <v>926312</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D16" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E16" s="12">
         <v>786.8</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="11">
+        <v>43349</v>
+      </c>
+      <c r="C17" s="10">
+        <v>925739</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="12">
+        <v>1091.8</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="11">
+        <v>43339</v>
+      </c>
+      <c r="C18" s="10">
+        <v>925134</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="12">
+        <v>1300</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="11">
+        <v>43340</v>
+      </c>
+      <c r="C19" s="10">
+        <v>925519</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="17">
-        <v>43349</v>
-      </c>
-      <c r="C3" s="13">
-        <v>925739</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="23">
-        <v>1091.8</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="E19" s="12">
+        <v>1076.4000000000001</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="17">
-        <v>43340</v>
-      </c>
-      <c r="C4" s="13">
-        <v>925519</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="B20" s="11">
+        <v>43332</v>
+      </c>
+      <c r="C20" s="10">
+        <v>924712</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E20" s="12">
         <v>1076.4000000000001</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="17">
-        <v>43339</v>
-      </c>
-      <c r="C5" s="13">
-        <v>925134</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="23">
-        <v>1300</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="13">
-        <v>924799</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="23">
-        <v>11459.91</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="17">
-        <v>43332</v>
-      </c>
-      <c r="C7" s="13">
-        <v>924712</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="23">
-        <v>1076.4000000000001</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="17">
-        <v>43327</v>
-      </c>
-      <c r="C8" s="13">
-        <v>924397</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="23">
-        <v>46812.86</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="19">
-        <v>43322</v>
-      </c>
-      <c r="C9" s="15">
-        <v>923984</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="25">
-        <v>1500</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="19">
-        <v>43318</v>
-      </c>
-      <c r="C10" s="15">
-        <v>923715</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="25">
-        <v>1435</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="19">
-        <v>43315</v>
-      </c>
-      <c r="C11" s="15">
-        <v>923679</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="25">
-        <v>8089.25</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="19">
-        <v>43313</v>
-      </c>
-      <c r="C12" s="15">
-        <v>923512</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="25">
-        <v>8230</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="19">
-        <v>43308</v>
-      </c>
-      <c r="C13" s="15">
-        <v>923150</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="25">
-        <v>6030</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="19">
-        <v>43306</v>
-      </c>
-      <c r="C14" s="15">
-        <v>922898</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="25">
-        <v>4585.5</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="19">
-        <v>43301</v>
-      </c>
-      <c r="C15" s="15">
-        <v>922709</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="25">
-        <v>744</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="19">
-        <v>43292</v>
-      </c>
-      <c r="C16" s="15">
-        <v>921645</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="25">
-        <v>7626.32</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="19">
-        <v>43291</v>
-      </c>
-      <c r="C17" s="15">
-        <v>921561</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="25">
-        <v>10748.76</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="19">
-        <v>43291</v>
-      </c>
-      <c r="C18" s="15">
-        <v>921560</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="25">
-        <v>2016</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="19">
-        <v>43290</v>
-      </c>
-      <c r="C19" s="15">
-        <v>921472</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="25">
-        <v>8794.5</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="19">
-        <v>43283</v>
-      </c>
-      <c r="C20" s="15">
-        <v>921166</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="25">
-        <v>768.8</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="3"/>
@@ -1385,20 +1439,20 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="19">
-        <v>43280</v>
-      </c>
-      <c r="C21" s="15">
-        <v>921068</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="25">
-        <v>15096.5</v>
+      <c r="A21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="10">
+        <v>924799</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="12">
+        <v>11459.91</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="3"/>
@@ -1423,20 +1477,20 @@
       <c r="Z21" s="3"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="19">
-        <v>43280</v>
-      </c>
-      <c r="C22" s="15">
-        <v>921043</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="25">
-        <v>4500</v>
+      <c r="A22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="11">
+        <v>43327</v>
+      </c>
+      <c r="C22" s="10">
+        <v>924397</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="12">
+        <v>46812.86</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
@@ -1461,1141 +1515,1281 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="11">
+        <v>43318</v>
+      </c>
+      <c r="C23" s="10">
+        <v>923715</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="12">
+        <v>1435</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="11">
+        <v>43322</v>
+      </c>
+      <c r="C24" s="10">
+        <v>923984</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1500</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="11">
+        <v>43313</v>
+      </c>
+      <c r="C25" s="10">
+        <v>923512</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="12">
+        <v>8230</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="11">
+        <v>43315</v>
+      </c>
+      <c r="C26" s="10">
+        <v>923679</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="12">
+        <v>8089.25</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="14">
+        <v>43307</v>
+      </c>
+      <c r="C27" s="13">
+        <v>14911</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="11">
+        <v>43306</v>
+      </c>
+      <c r="C28" s="10">
+        <v>922898</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="12">
+        <v>4585.5</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="11">
+        <v>43308</v>
+      </c>
+      <c r="C29" s="10">
+        <v>923150</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="12">
+        <v>6030</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="11">
+        <v>43301</v>
+      </c>
+      <c r="C30" s="10">
+        <v>922709</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="12">
+        <v>744</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="11">
+        <v>43292</v>
+      </c>
+      <c r="C31" s="10">
+        <v>921645</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="12">
+        <v>7626.32</v>
+      </c>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B32" s="11">
+        <v>43291</v>
+      </c>
+      <c r="C32" s="10">
+        <v>921561</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="12">
+        <v>10748.76</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11">
+        <v>43291</v>
+      </c>
+      <c r="C33" s="10">
+        <v>921560</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="12">
+        <v>2016</v>
+      </c>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="11">
+        <v>43290</v>
+      </c>
+      <c r="C34" s="10">
+        <v>921472</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="12">
+        <v>8794.5</v>
+      </c>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="11">
+        <v>43283</v>
+      </c>
+      <c r="C35" s="10">
+        <v>921166</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="12">
+        <v>768.8</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="11">
+        <v>43280</v>
+      </c>
+      <c r="C36" s="10">
+        <v>921068</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="12">
+        <v>15096.5</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="11">
+        <v>43278</v>
+      </c>
+      <c r="C37" s="10">
+        <v>920873</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="12">
+        <v>6030</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="11">
+        <v>43280</v>
+      </c>
+      <c r="C38" s="10">
+        <v>921043</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="12">
+        <v>4500</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="11">
         <v>43279</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C39" s="10">
         <v>920895</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D39" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E39" s="12">
         <v>10154.549999999999</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B40" s="11">
         <v>43279</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C40" s="10">
         <v>920874</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E40" s="12">
         <v>1225</v>
       </c>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="11">
+        <v>43271</v>
+      </c>
+      <c r="C41" s="10">
+        <v>920435</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="12">
+        <v>3815</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="11">
+        <v>43265</v>
+      </c>
+      <c r="C42" s="10">
+        <v>919875</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="12">
+        <v>9810</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="11">
+        <v>43265</v>
+      </c>
+      <c r="C43" s="10">
+        <v>919872</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="12">
+        <v>3000</v>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="11">
+        <v>43257</v>
+      </c>
+      <c r="C44" s="10">
+        <v>919431</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="12">
+        <v>6454.03</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="11">
+        <v>43250</v>
+      </c>
+      <c r="C45" s="10">
+        <v>918952</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="12">
+        <v>8794.5</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="11">
+        <v>43250</v>
+      </c>
+      <c r="C46" s="10">
+        <v>918973</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="12">
+        <v>3448.8</v>
+      </c>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="11">
+        <v>43244</v>
+      </c>
+      <c r="C47" s="10">
+        <v>918596</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="12">
+        <v>1435</v>
+      </c>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="11">
+        <v>43243</v>
+      </c>
+      <c r="C48" s="10">
+        <v>918491</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="12">
+        <v>2069.5</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="11">
+        <v>43237</v>
+      </c>
+      <c r="C49" s="10">
+        <v>917787</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="12">
+        <v>1500</v>
+      </c>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="11">
+        <v>43229</v>
+      </c>
+      <c r="C50" s="10">
+        <v>917095</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="12">
+        <v>6552.71</v>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="11">
+        <v>43220</v>
+      </c>
+      <c r="C51" s="10">
+        <v>916471</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="17">
+        <v>1091.8</v>
+      </c>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="11">
+        <v>43196</v>
+      </c>
+      <c r="C52" s="10">
+        <v>914826</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="12">
+        <v>10167.75</v>
+      </c>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="11">
+        <v>43171</v>
+      </c>
+      <c r="C53" s="10">
+        <v>913032</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="12">
+        <v>5214.3</v>
+      </c>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="11">
+        <v>43166</v>
+      </c>
+      <c r="C54" s="10">
+        <v>912670</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="12">
+        <v>12538.6</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="11">
+        <v>43159</v>
+      </c>
+      <c r="C55" s="10">
+        <v>912207</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55" s="12">
+        <v>5450</v>
+      </c>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="11">
+        <v>43158</v>
+      </c>
+      <c r="C56" s="10">
+        <v>912090</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="12">
+        <v>29408.5</v>
+      </c>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="11">
+        <v>43159</v>
+      </c>
+      <c r="C57" s="10">
+        <v>912163</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="12">
+        <v>6318</v>
+      </c>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="19">
-        <v>43278</v>
-      </c>
-      <c r="C25" s="15">
-        <v>920873</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="B58" s="11">
+        <v>43157</v>
+      </c>
+      <c r="C58" s="10">
+        <v>912049</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="12">
         <v>6030</v>
       </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" s="11">
+        <v>43136</v>
+      </c>
+      <c r="C59" s="10">
+        <v>910715</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="12">
+        <v>5059.2</v>
+      </c>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="11">
+        <v>43129</v>
+      </c>
+      <c r="C60" s="10">
+        <v>910308</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="12">
+        <v>8040</v>
+      </c>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="11">
+        <v>43129</v>
+      </c>
+      <c r="C61" s="10">
+        <v>910263</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="12">
+        <v>2840.4</v>
+      </c>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="11">
+        <v>43129</v>
+      </c>
+      <c r="C62" s="10">
+        <v>910268</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="12">
+        <v>8230</v>
+      </c>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="11">
+        <v>43126</v>
+      </c>
+      <c r="C63" s="10">
+        <v>910106</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="12">
+        <v>2183.6</v>
+      </c>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="19">
-        <v>43271</v>
-      </c>
-      <c r="C26" s="15">
-        <v>920435</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="B64" s="11">
+        <v>43124</v>
+      </c>
+      <c r="C64" s="10">
+        <v>909908</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="25">
-        <v>3815</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="19">
-        <v>43265</v>
-      </c>
-      <c r="C27" s="15">
-        <v>919875</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="25">
-        <v>9810</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+      <c r="E64" s="12">
+        <v>18863.5</v>
+      </c>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="18">
-        <v>43265</v>
-      </c>
-      <c r="C28" s="21">
-        <v>919872</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="24">
+      <c r="B65" s="11">
+        <v>43119</v>
+      </c>
+      <c r="C65" s="10">
+        <v>909591</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E65" s="12">
         <v>3000</v>
       </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="6">
-        <v>43257</v>
-      </c>
-      <c r="C29" s="7">
-        <v>919431</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="8">
-        <v>6454.03</v>
-      </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="6">
-        <v>43250</v>
-      </c>
-      <c r="C30" s="7">
-        <v>918973</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="8">
-        <v>3448.8</v>
-      </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="6">
-        <v>43250</v>
-      </c>
-      <c r="C31" s="7">
-        <v>918952</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="8">
-        <v>8794.5</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="11">
+        <v>43116</v>
+      </c>
+      <c r="C66" s="10">
+        <v>909387</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E66" s="12">
+        <v>796</v>
+      </c>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="11">
+        <v>43116</v>
+      </c>
+      <c r="C67" s="10">
+        <v>909411</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="12">
+        <v>5995</v>
+      </c>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="6">
-        <v>43244</v>
-      </c>
-      <c r="C32" s="7">
-        <v>918596</v>
-      </c>
-      <c r="D32" s="7" t="s">
+      <c r="B68" s="18">
+        <v>43112</v>
+      </c>
+      <c r="C68" s="19">
+        <v>909155</v>
+      </c>
+      <c r="D68" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="8">
-        <v>1435</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6">
-        <v>43243</v>
-      </c>
-      <c r="C33" s="7">
-        <v>918491</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="8">
-        <v>2069.5</v>
-      </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="6">
-        <v>43237</v>
-      </c>
-      <c r="C34" s="7">
-        <v>917787</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="8">
-        <v>1500</v>
-      </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="6">
-        <v>43229</v>
-      </c>
-      <c r="C35" s="7">
-        <v>917095</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="8">
-        <v>6552.71</v>
-      </c>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B36" s="6">
-        <v>43220</v>
-      </c>
-      <c r="C36" s="7">
-        <v>916471</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="E68" s="20">
+        <v>2670</v>
+      </c>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="18">
+        <v>43103</v>
+      </c>
+      <c r="C69" s="19">
+        <v>908483</v>
+      </c>
+      <c r="D69" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E69" s="20">
         <v>1091.8</v>
       </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="6">
-        <v>43196</v>
-      </c>
-      <c r="C37" s="7">
-        <v>914826</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="8">
-        <v>10167.75</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="6">
-        <v>43171</v>
-      </c>
-      <c r="C38" s="7">
-        <v>913032</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="8">
-        <v>5214.3</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="6">
-        <v>43166</v>
-      </c>
-      <c r="C39" s="7">
-        <v>912670</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="8">
-        <v>12538.6</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="6">
-        <v>43159</v>
-      </c>
-      <c r="C40" s="7">
-        <v>912207</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40" s="8">
-        <v>5450</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="6">
-        <v>43159</v>
-      </c>
-      <c r="C41" s="7">
-        <v>912163</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="8">
-        <v>6318</v>
-      </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="6">
-        <v>43158</v>
-      </c>
-      <c r="C42" s="7">
-        <v>912090</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="8">
-        <v>29408.5</v>
-      </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="6">
-        <v>43157</v>
-      </c>
-      <c r="C43" s="7">
-        <v>912049</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="8">
-        <v>6030</v>
-      </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="6">
-        <v>43136</v>
-      </c>
-      <c r="C44" s="7">
-        <v>910715</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="8">
-        <v>5059.2</v>
-      </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B45" s="6">
-        <v>43129</v>
-      </c>
-      <c r="C45" s="7">
-        <v>910308</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="8">
-        <v>8040</v>
-      </c>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="6">
-        <v>43129</v>
-      </c>
-      <c r="C46" s="7">
-        <v>910268</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="8">
-        <v>8230</v>
-      </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="6">
-        <v>43129</v>
-      </c>
-      <c r="C47" s="7">
-        <v>910263</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E47" s="8">
-        <v>2840.4</v>
-      </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" s="6">
-        <v>43126</v>
-      </c>
-      <c r="C48" s="7">
-        <v>910106</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="8">
-        <v>2183.6</v>
-      </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="6">
-        <v>43124</v>
-      </c>
-      <c r="C49" s="7">
-        <v>909908</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="8">
-        <v>18863.5</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="6">
-        <v>43119</v>
-      </c>
-      <c r="C50" s="7">
-        <v>909591</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="8">
-        <v>3000</v>
-      </c>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="6">
-        <v>43116</v>
-      </c>
-      <c r="C51" s="7">
-        <v>909411</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="8">
-        <v>5995</v>
-      </c>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B52" s="6">
-        <v>43116</v>
-      </c>
-      <c r="C52" s="7">
-        <v>909387</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="8">
-        <v>796</v>
-      </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B53" s="6">
-        <v>43112</v>
-      </c>
-      <c r="C53" s="10">
-        <v>909155</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="8">
-        <v>2670</v>
-      </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B54" s="6">
-        <v>43103</v>
-      </c>
-      <c r="C54" s="10">
-        <v>908483</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E54" s="8">
-        <v>1091.8</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B55" s="20">
-        <v>43307</v>
-      </c>
-      <c r="C55" s="22">
-        <v>14911</v>
-      </c>
-      <c r="D55" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="4"/>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="4"/>
+      <c r="A70" s="29"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="36"/>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="4"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="24"/>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="4"/>
+      <c r="A72" s="29"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="36"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="4"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="24"/>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="4"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="36"/>
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="4"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="24"/>
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="4"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="31"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="36"/>
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="4"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="24"/>
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="4"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="36"/>
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="4"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="4"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="36"/>
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="4"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="4"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="36"/>
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="4"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="24"/>
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="4"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="31"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="37"/>
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="4"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="24"/>
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="4"/>
+      <c r="A86" s="29"/>
+      <c r="B86" s="31"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="36"/>
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="4"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="24"/>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="4"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="36"/>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="4"/>
+      <c r="A89" s="21"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="24"/>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="4"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="31"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="36"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="4"/>
+      <c r="A91" s="21"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="24"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="4"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="31"/>
+      <c r="C92" s="33"/>
+      <c r="D92" s="33"/>
+      <c r="E92" s="36"/>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="4"/>
+      <c r="A93" s="21"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="24"/>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="4"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="36"/>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="4"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="23"/>
+      <c r="D95" s="23"/>
+      <c r="E95" s="24"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="4"/>
+      <c r="A96" s="29"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="36"/>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="4"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="22"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="24"/>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="4"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="36"/>
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="4"/>
+      <c r="A99" s="21"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="23"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="24"/>
       <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="4"/>
+      <c r="A100" s="29"/>
+      <c r="B100" s="31"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="36"/>
       <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="4"/>
+      <c r="A101" s="21"/>
+      <c r="B101" s="22"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="24"/>
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="4"/>
+      <c r="A102" s="29"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="36"/>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="4"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="23"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="24"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="4"/>
+      <c r="A104" s="29"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33"/>
+      <c r="E104" s="36"/>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="4"/>
+      <c r="A105" s="21"/>
+      <c r="B105" s="22"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="24"/>
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="4"/>
+      <c r="A106" s="29"/>
+      <c r="B106" s="31"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="36"/>
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="4"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="22"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="24"/>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="4"/>
+      <c r="A108" s="29"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="33"/>
+      <c r="D108" s="33"/>
+      <c r="E108" s="36"/>
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="4"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="24"/>
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="4"/>
+      <c r="A110" s="29"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="33"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="36"/>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="4"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="22"/>
+      <c r="C111" s="23"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="24"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="4"/>
+      <c r="A112" s="29"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="33"/>
+      <c r="D112" s="33"/>
+      <c r="E112" s="36"/>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="4"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="22"/>
+      <c r="C113" s="23"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="24"/>
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="4"/>
+      <c r="A114" s="29"/>
+      <c r="B114" s="31"/>
+      <c r="C114" s="33"/>
+      <c r="D114" s="33"/>
+      <c r="E114" s="36"/>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="4"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="23"/>
+      <c r="D115" s="23"/>
+      <c r="E115" s="24"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="4"/>
+      <c r="A116" s="29"/>
+      <c r="B116" s="31"/>
+      <c r="C116" s="33"/>
+      <c r="D116" s="33"/>
+      <c r="E116" s="36"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="4"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="22"/>
+      <c r="C117" s="23"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="24"/>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="4"/>
+      <c r="A118" s="29"/>
+      <c r="B118" s="31"/>
+      <c r="C118" s="34"/>
+      <c r="D118" s="33"/>
+      <c r="E118" s="36"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="4"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="22"/>
+      <c r="C119" s="23"/>
+      <c r="D119" s="23"/>
+      <c r="E119" s="24"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="4"/>
+      <c r="A120" s="29"/>
+      <c r="B120" s="31"/>
+      <c r="C120" s="34"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="36"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="4"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="24"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="4"/>
+      <c r="A122" s="30"/>
+      <c r="B122" s="32"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
       <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="4"/>
+      <c r="A123" s="25"/>
+      <c r="B123" s="26"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="28"/>
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>